<commit_message>
first test upload with 750k NC datapoints; awaiting publication
</commit_message>
<xml_diff>
--- a/scheduled_scripts/cuahsi/NC_Advanced.xlsx
+++ b/scheduled_scripts/cuahsi/NC_Advanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="753" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="891" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="422">
   <si>
     <t>How to Use this Guide</t>
   </si>
@@ -594,7 +594,7 @@
     <t>WaterPres_kPa</t>
   </si>
   <si>
-    <t>Pressure</t>
+    <t>Pressure, absolute</t>
   </si>
   <si>
     <t>kilopascal</t>
@@ -606,7 +606,7 @@
     <t>Field Observation</t>
   </si>
   <si>
-    <t>seconds</t>
+    <t>second</t>
   </si>
   <si>
     <t>Continuous</t>
@@ -696,9 +696,6 @@
     <t>Oxygen, dissolved</t>
   </si>
   <si>
-    <t>O2</t>
-  </si>
-  <si>
     <t>milligrams per liter</t>
   </si>
   <si>
@@ -732,6 +729,9 @@
     <t>Luminous Flux</t>
   </si>
   <si>
+    <t>LUX</t>
+  </si>
+  <si>
     <t>Light2_lux</t>
   </si>
   <si>
@@ -963,7 +963,7 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>UEno</t>
+    <t>NC_UEno</t>
   </si>
   <si>
     <t>East Eno River</t>
@@ -981,31 +981,31 @@
     <t>Stream</t>
   </si>
   <si>
-    <t>Eno</t>
+    <t>NC_Eno</t>
   </si>
   <si>
     <t>Eno River</t>
   </si>
   <si>
-    <t>Mud</t>
+    <t>NC_Mud</t>
   </si>
   <si>
     <t>Mud Tributary</t>
   </si>
   <si>
-    <t>NHC</t>
+    <t>NC_NHC</t>
   </si>
   <si>
     <t>New Hope Creek</t>
   </si>
   <si>
-    <t>UNHC</t>
+    <t>NC_UNHC</t>
   </si>
   <si>
     <t>Upper New Hope Creek</t>
   </si>
   <si>
-    <t>Stony</t>
+    <t>NC_Stony</t>
   </si>
   <si>
     <t>Stony Creek</t>
@@ -1116,6 +1116,36 @@
     <t>Link to additional metadata reference material.</t>
   </si>
   <si>
+    <t>ASU</t>
+  </si>
+  <si>
+    <t>Arizona State University</t>
+  </si>
+  <si>
+    <t>Campbell Scientific CR1000 Sonde Sensor Set Up</t>
+  </si>
+  <si>
+    <t>Nancy Grimm</t>
+  </si>
+  <si>
+    <t>480-965-4735</t>
+  </si>
+  <si>
+    <t>nbgrimm@asu.edu</t>
+  </si>
+  <si>
+    <t>School of Life Sciences, Arizona State University, Box 4501</t>
+  </si>
+  <si>
+    <t>Tempe</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>inlandWaters</t>
+  </si>
+  <si>
     <t>Duke</t>
   </si>
   <si>
@@ -1128,45 +1158,12 @@
     <t>Emily Bernhardt</t>
   </si>
   <si>
+    <t>919-660-7318</t>
+  </si>
+  <si>
     <t>ebernhar@duke.edu</t>
   </si>
   <si>
-    <t>Bernhardt, Emily S., et al. "The metabolic regimes of flowing waters." Limnology and Oceanography 63.S1 (2018): S99-S118.</t>
-  </si>
-  <si>
-    <t>ASU</t>
-  </si>
-  <si>
-    <t>Arizona State University</t>
-  </si>
-  <si>
-    <t>Campbell Scientific CR1000 Sonde Sensor Set Up</t>
-  </si>
-  <si>
-    <t>Nancy Grimm</t>
-  </si>
-  <si>
-    <t>480-965-4735</t>
-  </si>
-  <si>
-    <t>nbgrimm@asu.edu</t>
-  </si>
-  <si>
-    <t>School of Life Sciences, Arizona State University, Box 4501</t>
-  </si>
-  <si>
-    <t>Tempe</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>inlandWaters</t>
-  </si>
-  <si>
-    <t>919-660-7318</t>
-  </si>
-  <si>
     <t>Duke University, French Family Science Center, 124 Science Drive</t>
   </si>
   <si>
@@ -1587,13 +1584,19 @@
     <t>Text of the data qualifying comment.</t>
   </si>
   <si>
+    <t>Unflagged</t>
+  </si>
+  <si>
     <t>Interesting</t>
   </si>
   <si>
-    <t>Datapoint has been flagged by a user as interesting.</t>
+    <t>Datapoint has been flagged as interesting by a user.</t>
   </si>
   <si>
     <t>Questionable</t>
+  </si>
+  <si>
+    <t>Datapoint has been flagged as questionable by a user.</t>
   </si>
 </sst>
 </file>
@@ -1677,12 +1680,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1764,7 +1769,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1859,10 +1864,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -2217,7 +2218,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2244,53 +2245,53 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>366</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="25" t="s">
         <v>370</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>372</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="O1" s="25" t="s">
         <v>374</v>
       </c>
-      <c r="M1" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="O1" s="26" t="s">
+      <c r="P1" s="25" t="s">
         <v>375</v>
       </c>
-      <c r="P1" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q1" s="25" t="s">
-        <v>349</v>
+      <c r="Q1" s="24" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,13 +2305,13 @@
         <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>63</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>187</v>
@@ -2322,25 +2323,25 @@
         <v>63</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>60</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>187</v>
@@ -2404,19 +2405,19 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="D4" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>382</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>194</v>
@@ -2425,31 +2426,31 @@
         <v>68</v>
       </c>
       <c r="I4" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="J4" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="K4" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="L4" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="M4" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="N4" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="O4" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="Q4" s="23" t="s">
         <v>390</v>
-      </c>
-      <c r="Q4" s="23" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,13 +2464,13 @@
         <v>145</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>81</v>
@@ -2478,19 +2479,19 @@
         <v>81</v>
       </c>
       <c r="I5" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>392</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>393</v>
       </c>
       <c r="L5" s="0" t="s">
         <v>145</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N5" s="0" t="s">
         <v>81</v>
@@ -2501,8 +2502,8 @@
       <c r="P5" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="Q5" s="33" t="s">
-        <v>395</v>
+      <c r="Q5" s="32" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -2538,16 +2539,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>396</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,7 +2556,7 @@
         <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>63</v>
@@ -2568,14 +2569,14 @@
       <c r="A3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>331</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>344</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>344</v>
+      <c r="B3" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,10 +2587,10 @@
         <v>68</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>398</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,11 +2641,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>400</v>
+      <c r="B1" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,32 +2653,32 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>400</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>401</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,11 +2726,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>403</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2737,7 +2738,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>140</v>
@@ -2747,10 +2748,10 @@
       <c r="A3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>406</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="28" t="s">
+        <v>405</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2759,10 +2760,10 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>407</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2809,11 +2810,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>403</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>400</v>
+      <c r="B1" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,10 +2822,10 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2832,21 +2833,21 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>409</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,11 +2895,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>411</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2913,25 +2914,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>413</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,10 +2962,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2979,11 +2980,11 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>374</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>415</v>
+      <c r="B1" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3002,21 +3003,21 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>416</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,20 +3031,28 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
         <v>418</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>420</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>419</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3682,8 +3691,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3862,7 +3871,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
         <v>80</v>
       </c>
@@ -3923,7 +3932,7 @@
       <c r="G6" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="24" t="n">
+      <c r="H6" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3962,7 +3971,7 @@
       <c r="G7" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="24" t="n">
+      <c r="H7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="0" t="n">
@@ -4000,7 +4009,7 @@
       <c r="G8" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="24" t="n">
+      <c r="H8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="0" t="n">
@@ -4038,7 +4047,7 @@
       <c r="G9" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="H9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="0" t="n">
@@ -4076,7 +4085,7 @@
       <c r="G10" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="24" t="n">
+      <c r="H10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I10" s="0" t="n">
@@ -4114,7 +4123,7 @@
       <c r="G11" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="24" t="n">
+      <c r="H11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I11" s="0" t="n">
@@ -4152,7 +4161,7 @@
       <c r="G12" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="24" t="n">
+      <c r="H12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I12" s="0" t="n">
@@ -4190,7 +4199,7 @@
       <c r="G13" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="24" t="n">
+      <c r="H13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="0" t="n">
@@ -4217,10 +4226,10 @@
         <v>120</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>89</v>
@@ -4228,7 +4237,7 @@
       <c r="G14" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="24" t="n">
+      <c r="H14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="0" t="n">
@@ -4249,10 +4258,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>82</v>
@@ -4261,12 +4270,12 @@
         <v>88</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="24" t="n">
+      <c r="H15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="0" t="n">
@@ -4279,7 +4288,7 @@
         <v>92</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>-9999</v>
@@ -4287,7 +4296,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>95</v>
@@ -4299,12 +4308,12 @@
         <v>96</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="24" t="n">
+      <c r="H16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I16" s="0" t="n">
@@ -4317,7 +4326,7 @@
         <v>92</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>-9999</v>
@@ -4325,16 +4334,16 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="E17" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>89</v>
@@ -4342,7 +4351,7 @@
       <c r="G17" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="24" t="n">
+      <c r="H17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="0" t="n">
@@ -4363,10 +4372,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>132</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>82</v>
@@ -4380,7 +4389,7 @@
       <c r="G18" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="24" t="n">
+      <c r="H18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="0" t="n">
@@ -4393,7 +4402,7 @@
         <v>92</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>-9999</v>
@@ -4404,7 +4413,7 @@
         <v>133</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>82</v>
@@ -4418,7 +4427,7 @@
       <c r="G19" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="24" t="n">
+      <c r="H19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="0" t="n">
@@ -4431,7 +4440,7 @@
         <v>92</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>-9999</v>
@@ -4456,7 +4465,7 @@
       <c r="G20" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="24" t="n">
+      <c r="H20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="0" t="n">
@@ -4469,7 +4478,7 @@
         <v>92</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M20" s="0" t="n">
         <v>-9999</v>
@@ -4493,8 +4502,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4510,13 +4519,13 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4704,8 +4713,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -4732,49 +4741,49 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="26" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5134,10 +5143,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5161,55 +5170,55 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="R1" s="27" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5438,300 +5447,370 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="28" t="s">
         <v>262</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="E6" s="21"/>
+      <c r="F6" s="28" t="s">
         <v>264</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="G6" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="H6" s="28" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
-      <c r="N7" s="21"/>
+      <c r="I6" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="L6" s="29" t="n">
+        <v>85287</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="L7" s="29" t="n">
+        <v>27708</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="R7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>268</v>
+      <c r="B8" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>281</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="L8" s="29" t="n">
+        <v>32611</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="G8" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="L8" s="30" t="n">
-        <v>85287</v>
-      </c>
-      <c r="M8" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P8" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q8" s="29" t="s">
-        <v>83</v>
-      </c>
+      <c r="O8" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="29" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>262</v>
+      <c r="B9" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>289</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>263</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>265</v>
-      </c>
-      <c r="I9" s="29" t="s">
+      <c r="F9" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="J9" s="28" t="s">
         <v>278</v>
       </c>
-      <c r="J9" s="29" t="s">
-        <v>279</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="L9" s="30" t="n">
-        <v>27708</v>
-      </c>
-      <c r="M9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="O9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P9" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q9" s="29" t="s">
+      <c r="K9" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q9" s="28" t="s">
         <v>83</v>
       </c>
       <c r="R9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="29" t="s">
-        <v>281</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>282</v>
+      <c r="B10" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>297</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="E10" s="21"/>
-      <c r="F10" s="29" t="s">
-        <v>283</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="L10" s="30" t="n">
-        <v>32611</v>
-      </c>
-      <c r="M10" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N10" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="O10" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P10" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q10" s="29" t="s">
+      <c r="F10" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="L10" s="29" t="n">
+        <v>53705</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q10" s="28" t="s">
         <v>83</v>
       </c>
       <c r="R10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="29" t="s">
-        <v>289</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>290</v>
+      <c r="B11" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>305</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>279</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>295</v>
-      </c>
-      <c r="L11" s="30" t="s">
-        <v>296</v>
-      </c>
-      <c r="M11" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N11" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="O11" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P11" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q11" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="R11" s="21"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="29" t="s">
-        <v>297</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>298</v>
+        <v>83</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q11" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>311</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="29" t="s">
-        <v>299</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>300</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>304</v>
-      </c>
-      <c r="L12" s="30" t="n">
-        <v>53705</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="N12" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="O12" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P12" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q12" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="R12" s="21"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="21" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>83</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>308</v>
+      <c r="H13" s="31" t="s">
+        <v>319</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>83</v>
@@ -5740,7 +5819,7 @@
         <v>83</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="O13" s="0" t="s">
         <v>83</v>
@@ -5754,31 +5833,31 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="21" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>83</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>313</v>
+        <v>83</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="31" t="s">
-        <v>314</v>
+      <c r="H14" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>315</v>
+        <v>83</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>316</v>
+        <v>83</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>83</v>
@@ -5787,7 +5866,7 @@
         <v>83</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="O14" s="0" t="s">
         <v>83</v>
@@ -5801,31 +5880,31 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="21" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>319</v>
+        <v>83</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="32" t="s">
-        <v>320</v>
+      <c r="H15" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>321</v>
+        <v>83</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>322</v>
+        <v>83</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>83</v>
@@ -5834,7 +5913,7 @@
         <v>83</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="O15" s="0" t="s">
         <v>83</v>
@@ -5846,106 +5925,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="P16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q16" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="21" t="s">
-        <v>325</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="N17" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="O17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="P17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q17" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" display="ebernhar@duke.edu"/>
-    <hyperlink ref="H13" r:id="rId2" display="amber.ulseth@epfl.ch"/>
-    <hyperlink ref="H15" r:id="rId3" display="jake.hosen@yale.edu"/>
+    <hyperlink ref="H11" r:id="rId1" display="amber.ulseth@epfl.ch"/>
+    <hyperlink ref="H13" r:id="rId2" display="jake.hosen@yale.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5965,7 +5951,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5981,14 +5967,14 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>327</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>328</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6002,7 +5988,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6010,13 +5996,13 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>332</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="4" s="21" customFormat="true" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6024,13 +6010,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="D4" s="23" t="s">
         <v>335</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6044,7 +6030,7 @@
         <v>81</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -6082,20 +6068,20 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="25" t="s">
         <v>340</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6123,16 +6109,16 @@
         <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>343</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>344</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
@@ -6143,19 +6129,19 @@
         <v>67</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="D4" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>336</v>
-      </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>347</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6212,14 +6198,14 @@
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>349</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>350</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6255,13 +6241,13 @@
         <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6269,68 +6255,68 @@
         <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>355</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="29" t="s">
+      <c r="D6" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="D6" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="29" t="s">
+      <c r="D7" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="D7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="29" t="s">
+      <c r="D8" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="D8" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="29" t="s">
+      <c r="D9" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="D9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="29" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalizing cuahsi sync script
</commit_message>
<xml_diff>
--- a/scheduled_scripts/cuahsi/NC_Advanced.xlsx
+++ b/scheduled_scripts/cuahsi/NC_Advanced.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="422">
   <si>
     <t>How to Use this Guide</t>
   </si>
@@ -1769,7 +1769,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1910,6 +1910,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2965,7 +2969,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3032,8 +3036,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>145</v>
+      <c r="B6" s="35" t="n">
+        <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>417</v>
@@ -5145,8 +5149,8 @@
   </sheetPr>
   <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6182,8 +6186,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>